<commit_message>
ks2 + ks3 + some works
</commit_message>
<xml_diff>
--- a/scripts/reports/My_spec.xlsx
+++ b/scripts/reports/My_spec.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Наименование работ и материалов</t>
   </si>
@@ -193,55 +193,28 @@
     <t>Монтажные и пусконаладочные работы по разделу 1:</t>
   </si>
   <si>
-    <t>olalaTest</t>
-  </si>
-  <si>
-    <t>olalala</t>
-  </si>
-  <si>
-    <t>gggg</t>
+    <t>название</t>
   </si>
   <si>
     <t>шт</t>
   </si>
   <si>
-    <t>Итого за монтажные и пусконаладочные работы по разделу 1:</t>
+    <t>Итого</t>
   </si>
   <si>
     <t>Оборудование и материалы по разделу 1:</t>
   </si>
   <si>
-    <t>olala2</t>
-  </si>
-  <si>
-    <t>olalala2</t>
-  </si>
-  <si>
-    <t>Итого за оборудование и материалы по разделу 1:</t>
-  </si>
-  <si>
-    <t>Итого за раздел 1. система  автоматической пожарной сигнализации и оповещения и управления эвакуацией людей при пожаре (апс и соуэ)</t>
+    <t>Итого по разделу</t>
   </si>
   <si>
     <t>Раздел TST</t>
   </si>
   <si>
-    <t>Монтажные и пусконаладочные работы по разделу :</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Итого за монтажные и пусконаладочные работы по разделу :</t>
-  </si>
-  <si>
-    <t>Оборудование и материалы по разделу :</t>
-  </si>
-  <si>
-    <t>Итого за оборудование и материалы по разделу :</t>
-  </si>
-  <si>
-    <t>Итого за раздел</t>
+    <t>Подраздел:</t>
+  </si>
+  <si>
+    <t>Итого:</t>
   </si>
 </sst>
 </file>
@@ -909,135 +882,135 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H4" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5">
-        <v>3000</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="9" r="5" spans="1:10">
       <c r="A5" s="12">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>57</v>
-      </c>
       <c r="H5" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J5" s="5">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="9" r="6" spans="1:10">
       <c r="A6" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="9" r="7" spans="1:10">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="9" r="8" spans="1:10">
+      <c r="A8" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.15" r="9" spans="1:10">
+      <c r="A9" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="5">
-        <v>10</v>
-      </c>
-      <c r="I6" s="5">
-        <v>20</v>
-      </c>
-      <c r="J6" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="9" r="7" spans="1:10">
-      <c r="A7" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="5">
-        <v>3400</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.15" r="8" spans="1:10">
-      <c r="A8" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row customHeight="1" ht="9" r="9" spans="1:10">
-      <c r="A9" s="12">
-        <v>42</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
-        <v>30</v>
-      </c>
-      <c r="J9" s="5">
-        <v>30</v>
-      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row customHeight="1" ht="9" r="10" spans="1:10">
       <c r="A10" s="12">
-        <v>43</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B10" s="12"/>
       <c r="C10" s="13" t="s">
-        <v>61</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H10" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J10" s="5">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="9" r="11" spans="1:10">
       <c r="A11" s="20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -1048,12 +1021,12 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="5">
-        <v>1030</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="12.15" r="12" spans="1:10">
       <c r="A12" s="19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -1064,12 +1037,12 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="8">
-        <v>4430</v>
+        <v>5</v>
       </c>
     </row>
     <row customHeight="1" ht="31.5" r="13" spans="1:10">
       <c r="A13" s="24" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -1083,7 +1056,7 @@
     </row>
     <row customHeight="1" ht="12.15" r="14" spans="1:10">
       <c r="A14" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -1096,32 +1069,32 @@
       <c r="J14" s="18"/>
     </row>
     <row customHeight="1" ht="9" r="15" spans="1:10">
-      <c r="A15" s="12" t="s">
-        <v>66</v>
+      <c r="A15" s="12">
+        <v>6</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="11" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="9" r="16" spans="1:10">
       <c r="A16" s="20" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -1132,12 +1105,12 @@
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
       <c r="J16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="12.15" r="17" spans="1:10">
       <c r="A17" s="18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1150,32 +1123,32 @@
       <c r="J17" s="18"/>
     </row>
     <row customHeight="1" ht="9" r="18" spans="1:10">
-      <c r="A18" s="12" t="s">
-        <v>66</v>
+      <c r="A18" s="12">
+        <v>7</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="11" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="9" r="19" spans="1:10">
       <c r="A19" s="20" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -1186,12 +1159,12 @@
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
       <c r="J19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="12.15" r="20" spans="1:10">
       <c r="A20" s="19" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1202,7 +1175,7 @@
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="12.15" r="21" spans="1:10">
@@ -1218,7 +1191,7 @@
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
       <c r="J21" s="6">
-        <v>354.40000000000003</v>
+        <v>0.56</v>
       </c>
     </row>
     <row customHeight="1" ht="12.15" r="22" spans="1:10">
@@ -1234,7 +1207,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="7">
-        <v>4784.4</v>
+        <v>9.072000000000001</v>
       </c>
     </row>
     <row customHeight="1" ht="9" r="23" spans="1:10">
@@ -1267,12 +1240,12 @@
   </sheetData>
   <mergeCells count="24111111">
     <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A8:I8"/>
     <mergeCell ref="A22:I22"/>
     <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A14:J14"/>
@@ -1292,10 +1265,10 @@
     <mergeCell ref="A12:I12"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>

</xml_diff>